<commit_message>
syazwan update s10 tc daily n weekly
</commit_message>
<xml_diff>
--- a/Excel Files/Scenario 10/S10-TC043-Upload WIP Adjustment.xlsx
+++ b/Excel Files/Scenario 10/S10-TC043-Upload WIP Adjustment.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="55">
   <si>
     <t>WIP Stock Adjustment</t>
   </si>
@@ -186,6 +186,18 @@
   </si>
   <si>
     <t>30 Oct 2023</t>
+  </si>
+  <si>
+    <t>ZUpna1219AS1</t>
+  </si>
+  <si>
+    <t>PNABU-L3-ZU-022</t>
+  </si>
+  <si>
+    <t>ZUpna-1219AS-1</t>
+  </si>
+  <si>
+    <t>25 Nov 2023</t>
   </si>
 </sst>
 </file>
@@ -694,16 +706,16 @@
     </row>
     <row ht="14.4" r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D4" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E4" t="s">
         <v>13</v>
@@ -715,7 +727,7 @@
         <v>12</v>
       </c>
       <c r="H4" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="I4" t="n">
         <v>66.0</v>

</xml_diff>